<commit_message>
add a column for room tags
</commit_message>
<xml_diff>
--- a/residents_exporter/template.xlsx
+++ b/residents_exporter/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daily-work\residents_exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>序号</t>
   </si>
@@ -44,6 +44,10 @@
   </si>
   <si>
     <t>情况说明：西街居委{unit_addr}楼共{num_rooms}户,{num_residents}人居住，其中**人已集中隔离，人员全部召回，目前在本楼道**人。</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>房屋标签</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -465,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -479,10 +483,11 @@
     <col min="4" max="4" width="22" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -492,7 +497,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -502,7 +507,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -521,14 +526,18 @@
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add --simple-address and --no-room-tag
</commit_message>
<xml_diff>
--- a/residents_exporter/template.xlsx
+++ b/residents_exporter/template.xlsx
@@ -471,14 +471,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="22" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>

</xml_diff>